<commit_message>
Updated project-mgmt-template with difficulty level
</commit_message>
<xml_diff>
--- a/project-management-template.xlsx
+++ b/project-management-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cnaik1\OneDrive - Intel Corporation\Desktop\scholarship\udacity-resources\building-a-ci-cd-pipeline\project\flask-sklearn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B66A20B7-95DF-4A8B-9CB3-6B5F316A7FC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B4C8B1-B4B6-4A47-A904-07B0D4A72CC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
   <si>
     <t>Week</t>
   </si>
@@ -50,9 +50,6 @@
   </si>
   <si>
     <t>Testing</t>
-  </si>
-  <si>
-    <t>Backend Ready for QA</t>
   </si>
   <si>
     <t>Run flask app with prediction</t>
@@ -99,13 +96,19 @@
   <si>
     <t>Submit the project</t>
   </si>
+  <si>
+    <t>easy</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -195,15 +198,9 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -213,6 +210,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,10 +434,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AB1003"/>
+  <dimension ref="A1:AB1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -456,11 +459,11 @@
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="14" t="s">
-        <v>13</v>
+      <c r="F1" s="13" t="s">
+        <v>12</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
@@ -486,20 +489,22 @@
       <c r="AB1" s="4"/>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A2" s="15">
+      <c r="A2" s="23">
         <v>2022</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="11">
-        <v>44814</v>
+      <c r="C2" s="24">
+        <v>44845</v>
       </c>
-      <c r="D2" s="13" t="s">
-        <v>12</v>
+      <c r="D2" s="12" t="s">
+        <v>11</v>
       </c>
       <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
+      <c r="F2" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
@@ -524,16 +529,18 @@
       <c r="AB2" s="6"/>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A3" s="15"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="11">
-        <v>44814</v>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="24">
+        <v>44845</v>
       </c>
-      <c r="D3" s="13" t="s">
-        <v>14</v>
+      <c r="D3" s="12" t="s">
+        <v>13</v>
       </c>
       <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
+      <c r="F3" s="12" t="s">
+        <v>25</v>
+      </c>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
@@ -558,16 +565,18 @@
       <c r="AB3" s="6"/>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A4" s="15"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="11">
-        <v>44814</v>
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="24">
+        <v>44845</v>
       </c>
-      <c r="D4" s="13" t="s">
-        <v>15</v>
+      <c r="D4" s="12" t="s">
+        <v>14</v>
       </c>
       <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
+      <c r="F4" s="12" t="s">
+        <v>25</v>
+      </c>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
@@ -592,16 +601,18 @@
       <c r="AB4" s="6"/>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="11">
-        <v>44814</v>
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="24">
+        <v>44845</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="11" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="5"/>
-      <c r="F5" s="6"/>
+      <c r="F5" s="12" t="s">
+        <v>25</v>
+      </c>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -626,18 +637,20 @@
       <c r="AB5" s="6"/>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A6" s="15"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="11">
-        <v>44814</v>
+      <c r="A6" s="23"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="24">
+        <v>44845</v>
       </c>
-      <c r="D6" s="16" t="s">
-        <v>16</v>
+      <c r="D6" s="14" t="s">
+        <v>15</v>
       </c>
-      <c r="E6" s="12" t="s">
-        <v>11</v>
+      <c r="E6" s="11" t="s">
+        <v>10</v>
       </c>
-      <c r="F6" s="6"/>
+      <c r="F6" s="12" t="s">
+        <v>26</v>
+      </c>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -662,16 +675,18 @@
       <c r="AB6" s="6"/>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A7" s="15"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="11">
-        <v>44814</v>
+      <c r="A7" s="23"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="24">
+        <v>44845</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="11" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="5"/>
-      <c r="F7" s="6"/>
+      <c r="F7" s="12" t="s">
+        <v>25</v>
+      </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -696,15 +711,17 @@
       <c r="AB7" s="6"/>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="11">
-        <v>44814</v>
+      <c r="A8" s="23"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="24">
+        <v>44845</v>
       </c>
-      <c r="D8" s="17" t="s">
-        <v>17</v>
+      <c r="D8" s="15" t="s">
+        <v>16</v>
       </c>
-      <c r="F8" s="6"/>
+      <c r="F8" s="12" t="s">
+        <v>26</v>
+      </c>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -729,16 +746,18 @@
       <c r="AB8" s="6"/>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="11">
-        <v>44814</v>
+      <c r="A9" s="23"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="24">
+        <v>44845</v>
       </c>
-      <c r="D9" s="18" t="s">
-        <v>18</v>
+      <c r="D9" s="16" t="s">
+        <v>17</v>
       </c>
       <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
+      <c r="F9" s="12" t="s">
+        <v>25</v>
+      </c>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -763,16 +782,18 @@
       <c r="AB9" s="6"/>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A10" s="15"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="11">
-        <v>44814</v>
+      <c r="A10" s="23"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="24">
+        <v>44845</v>
       </c>
-      <c r="D10" s="19" t="s">
-        <v>19</v>
+      <c r="D10" s="17" t="s">
+        <v>18</v>
       </c>
       <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
+      <c r="F10" s="12" t="s">
+        <v>26</v>
+      </c>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -797,16 +818,18 @@
       <c r="AB10" s="6"/>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A11" s="15"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="11">
-        <v>44814</v>
+      <c r="A11" s="23"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="24">
+        <v>44845</v>
       </c>
-      <c r="D11" s="20" t="s">
-        <v>20</v>
+      <c r="D11" s="18" t="s">
+        <v>19</v>
       </c>
       <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
+      <c r="F11" s="12" t="s">
+        <v>26</v>
+      </c>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -831,16 +854,18 @@
       <c r="AB11" s="6"/>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A12" s="15"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="11">
-        <v>44814</v>
+      <c r="A12" s="23"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="24">
+        <v>44845</v>
       </c>
-      <c r="D12" s="21" t="s">
-        <v>21</v>
+      <c r="D12" s="19" t="s">
+        <v>20</v>
       </c>
       <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
+      <c r="F12" s="12" t="s">
+        <v>25</v>
+      </c>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
@@ -865,16 +890,18 @@
       <c r="AB12" s="6"/>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A13" s="15"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="11">
-        <v>44814</v>
+      <c r="A13" s="23"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="24">
+        <v>44845</v>
       </c>
-      <c r="D13" s="22" t="s">
-        <v>22</v>
+      <c r="D13" s="20" t="s">
+        <v>21</v>
       </c>
       <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
+      <c r="F13" s="12" t="s">
+        <v>25</v>
+      </c>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
@@ -899,16 +926,18 @@
       <c r="AB13" s="6"/>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A14" s="15"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="11">
-        <v>44814</v>
+      <c r="A14" s="23"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="24">
+        <v>44846</v>
       </c>
-      <c r="D14" s="23" t="s">
-        <v>23</v>
+      <c r="D14" s="21" t="s">
+        <v>22</v>
       </c>
       <c r="E14" s="5"/>
-      <c r="F14" s="6"/>
+      <c r="F14" s="12" t="s">
+        <v>25</v>
+      </c>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
@@ -933,16 +962,18 @@
       <c r="AB14" s="6"/>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A15" s="15"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="11">
-        <v>44814</v>
+      <c r="A15" s="23"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="24">
+        <v>44846</v>
       </c>
-      <c r="D15" s="24" t="s">
-        <v>24</v>
+      <c r="D15" s="22" t="s">
+        <v>23</v>
       </c>
       <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
+      <c r="F15" s="12" t="s">
+        <v>25</v>
+      </c>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
@@ -967,79 +998,73 @@
       <c r="AB15" s="6"/>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A16" s="15"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="11">
-        <v>44814</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
-      <c r="N16" s="6"/>
-      <c r="O16" s="6"/>
-      <c r="P16" s="6"/>
-      <c r="Q16" s="6"/>
-      <c r="R16" s="6"/>
-      <c r="S16" s="6"/>
-      <c r="T16" s="6"/>
-      <c r="U16" s="6"/>
-      <c r="V16" s="6"/>
-      <c r="W16" s="6"/>
-      <c r="X16" s="6"/>
-      <c r="Y16" s="6"/>
-      <c r="Z16" s="6"/>
-      <c r="AA16" s="6"/>
-      <c r="AB16" s="6"/>
-    </row>
-    <row r="17" spans="3:28" x14ac:dyDescent="0.2">
-      <c r="C17" s="7"/>
-      <c r="D17" s="8" t="s">
+      <c r="C16" s="7"/>
+      <c r="D16" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E16" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="9"/>
-      <c r="P17" s="9"/>
-      <c r="Q17" s="9"/>
-      <c r="R17" s="9"/>
-      <c r="S17" s="9"/>
-      <c r="T17" s="9"/>
-      <c r="U17" s="9"/>
-      <c r="V17" s="9"/>
-      <c r="W17" s="9"/>
-      <c r="X17" s="9"/>
-      <c r="Y17" s="9"/>
-      <c r="Z17" s="9"/>
-      <c r="AA17" s="9"/>
-      <c r="AB17" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="9"/>
+      <c r="T16" s="9"/>
+      <c r="U16" s="9"/>
+      <c r="V16" s="9"/>
+      <c r="W16" s="9"/>
+      <c r="X16" s="9"/>
+      <c r="Y16" s="9"/>
+      <c r="Z16" s="9"/>
+      <c r="AA16" s="9"/>
+      <c r="AB16" s="9"/>
+    </row>
+    <row r="17" spans="3:28" x14ac:dyDescent="0.2">
+      <c r="C17" s="10"/>
+      <c r="D17" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="6"/>
+      <c r="T17" s="6"/>
+      <c r="U17" s="6"/>
+      <c r="V17" s="6"/>
+      <c r="W17" s="6"/>
+      <c r="X17" s="6"/>
+      <c r="Y17" s="6"/>
+      <c r="Z17" s="6"/>
+      <c r="AA17" s="6"/>
+      <c r="AB17" s="6"/>
     </row>
     <row r="18" spans="3:28" x14ac:dyDescent="0.2">
       <c r="C18" s="10"/>
-      <c r="D18" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
@@ -1066,8 +1091,8 @@
     </row>
     <row r="19" spans="3:28" x14ac:dyDescent="0.2">
       <c r="C19" s="10"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
@@ -28616,38 +28641,10 @@
       <c r="AA1002" s="6"/>
       <c r="AB1002" s="6"/>
     </row>
-    <row r="1003" spans="3:28" x14ac:dyDescent="0.2">
-      <c r="C1003" s="10"/>
-      <c r="D1003" s="6"/>
-      <c r="E1003" s="6"/>
-      <c r="F1003" s="6"/>
-      <c r="G1003" s="6"/>
-      <c r="H1003" s="6"/>
-      <c r="I1003" s="6"/>
-      <c r="J1003" s="6"/>
-      <c r="K1003" s="6"/>
-      <c r="L1003" s="6"/>
-      <c r="M1003" s="6"/>
-      <c r="N1003" s="6"/>
-      <c r="O1003" s="6"/>
-      <c r="P1003" s="6"/>
-      <c r="Q1003" s="6"/>
-      <c r="R1003" s="6"/>
-      <c r="S1003" s="6"/>
-      <c r="T1003" s="6"/>
-      <c r="U1003" s="6"/>
-      <c r="V1003" s="6"/>
-      <c r="W1003" s="6"/>
-      <c r="X1003" s="6"/>
-      <c r="Y1003" s="6"/>
-      <c r="Z1003" s="6"/>
-      <c r="AA1003" s="6"/>
-      <c r="AB1003" s="6"/>
-    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A2:A16"/>
-    <mergeCell ref="B2:B16"/>
+    <mergeCell ref="A2:A15"/>
+    <mergeCell ref="B2:B15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>